<commit_message>
Recalibrate CSC parameters based on ATB 2023 data
</commit_message>
<xml_diff>
--- a/InputData/elec/SoCtMbCtbDP/Shr of Costs that Must be Covered to be Deemed Profitable.xlsx
+++ b/InputData/elec/SoCtMbCtbDP/Shr of Costs that Must be Covered to be Deemed Profitable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\SoCtMbCtBDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\SoCtMbCtbDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59481EF6-97A0-49B9-97FC-8B00E4292FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CF41B4-27AD-42C6-B841-9FDDA9AD063A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11295" yWindow="6330" windowWidth="21840" windowHeight="9120" xr2:uid="{5E78EF81-321F-43F5-B343-4E83A6575A8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5E78EF81-321F-43F5-B343-4E83A6575A8A}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -197,9 +197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -237,7 +237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -343,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -546,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -554,7 +554,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -578,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -594,7 +594,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -610,7 +610,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -618,7 +618,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,7 +634,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,7 +642,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -658,7 +658,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -690,7 +690,7 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -698,7 +698,7 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +714,7 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use higher value for plant types early in learning curve
</commit_message>
<xml_diff>
--- a/InputData/elec/SoCtMbCtbDP/Shr of Costs that Must be Covered to be Deemed Profitable.xlsx
+++ b/InputData/elec/SoCtMbCtbDP/Shr of Costs that Must be Covered to be Deemed Profitable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\SoCtMbCtbDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\SoCtMbCtbDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CE7B47-9F60-4A8D-8DB6-1D03DBAFE5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478A7CC8-9EF5-461D-B79F-B9983E4209DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="1140" windowWidth="21690" windowHeight="18000" activeTab="1" xr2:uid="{5E78EF81-321F-43F5-B343-4E83A6575A8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{5E78EF81-321F-43F5-B343-4E83A6575A8A}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -497,14 +497,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -525,15 +525,15 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+      <selection activeCell="B19" sqref="B19:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -541,7 +541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -549,7 +549,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -557,7 +557,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -565,7 +565,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -573,7 +573,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -581,7 +581,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -589,7 +589,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -597,7 +597,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -605,7 +605,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -613,7 +613,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -621,7 +621,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -629,7 +629,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -637,7 +637,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -645,7 +645,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -653,7 +653,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -661,7 +661,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -669,7 +669,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -677,60 +677,60 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
       <c r="B24">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
       <c r="B25">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update share of costs that must be covered to be deemed profitable for dispatchable plants
</commit_message>
<xml_diff>
--- a/InputData/elec/SoCtMbCtbDP/Shr of Costs that Must be Covered to be Deemed Profitable.xlsx
+++ b/InputData/elec/SoCtMbCtbDP/Shr of Costs that Must be Covered to be Deemed Profitable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\SoCtMbCtbDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us-analysis\InputData\elec\SoCtMbCtbDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3800032A-20A2-44F8-A411-B32857CD437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C2FD9E-EFCC-4DF9-82F0-7BE08C7CAA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5E78EF81-321F-43F5-B343-4E83A6575A8A}"/>
   </bookViews>
@@ -559,7 +559,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B18" sqref="B18:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>